<commit_message>
Just worked out that OpenModel is row-wise...
</commit_message>
<xml_diff>
--- a/dat_canopy_2021.xlsx
+++ b/dat_canopy_2021.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N366"/>
+  <dimension ref="A1:P366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,6 +428,16 @@
           <t>fTemp</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>root_depth</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -471,6 +481,12 @@
       </c>
       <c r="N2">
         <v>1e-005</v>
+      </c>
+      <c r="O2">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P2">
+        <v>0.02</v>
       </c>
     </row>
     <row r="3">
@@ -516,6 +532,12 @@
       <c r="N3">
         <v>1e-005</v>
       </c>
+      <c r="O3">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P3">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -560,6 +582,12 @@
       <c r="N4">
         <v>1e-005</v>
       </c>
+      <c r="O4">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P4">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -604,6 +632,12 @@
       <c r="N5">
         <v>1e-005</v>
       </c>
+      <c r="O5">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P5">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -648,6 +682,12 @@
       <c r="N6">
         <v>1e-005</v>
       </c>
+      <c r="O6">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P6">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -692,6 +732,12 @@
       <c r="N7">
         <v>1e-005</v>
       </c>
+      <c r="O7">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P7">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -736,6 +782,12 @@
       <c r="N8">
         <v>1e-005</v>
       </c>
+      <c r="O8">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P8">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -780,6 +832,12 @@
       <c r="N9">
         <v>1e-005</v>
       </c>
+      <c r="O9">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P9">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -823,6 +881,12 @@
       </c>
       <c r="N10">
         <v>1e-005</v>
+      </c>
+      <c r="O10">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P10">
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
@@ -868,6 +932,12 @@
       <c r="N11">
         <v>1e-005</v>
       </c>
+      <c r="O11">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P11">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -912,6 +982,12 @@
       <c r="N12">
         <v>1e-005</v>
       </c>
+      <c r="O12">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P12">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -956,6 +1032,12 @@
       <c r="N13">
         <v>1e-005</v>
       </c>
+      <c r="O13">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P13">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -1000,6 +1082,12 @@
       <c r="N14">
         <v>1e-005</v>
       </c>
+      <c r="O14">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P14">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -1044,6 +1132,12 @@
       <c r="N15">
         <v>1e-005</v>
       </c>
+      <c r="O15">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P15">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -1088,6 +1182,12 @@
       <c r="N16">
         <v>1e-005</v>
       </c>
+      <c r="O16">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P16">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -1132,6 +1232,12 @@
       <c r="N17">
         <v>1e-005</v>
       </c>
+      <c r="O17">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P17">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -1176,6 +1282,12 @@
       <c r="N18">
         <v>1e-005</v>
       </c>
+      <c r="O18">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P18">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -1220,6 +1332,12 @@
       <c r="N19">
         <v>1e-005</v>
       </c>
+      <c r="O19">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P19">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -1264,6 +1382,12 @@
       <c r="N20">
         <v>1e-005</v>
       </c>
+      <c r="O20">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P20">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1308,6 +1432,12 @@
       <c r="N21">
         <v>1e-005</v>
       </c>
+      <c r="O21">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P21">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -1352,6 +1482,12 @@
       <c r="N22">
         <v>1e-005</v>
       </c>
+      <c r="O22">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P22">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1396,6 +1532,12 @@
       <c r="N23">
         <v>1e-005</v>
       </c>
+      <c r="O23">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P23">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -1440,6 +1582,12 @@
       <c r="N24">
         <v>1e-005</v>
       </c>
+      <c r="O24">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P24">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -1484,6 +1632,12 @@
       <c r="N25">
         <v>1e-005</v>
       </c>
+      <c r="O25">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P25">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -1528,6 +1682,12 @@
       <c r="N26">
         <v>1e-005</v>
       </c>
+      <c r="O26">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P26">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -1572,6 +1732,12 @@
       <c r="N27">
         <v>1e-005</v>
       </c>
+      <c r="O27">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P27">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -1616,6 +1782,12 @@
       <c r="N28">
         <v>1e-005</v>
       </c>
+      <c r="O28">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P28">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -1660,6 +1832,12 @@
       <c r="N29">
         <v>1e-005</v>
       </c>
+      <c r="O29">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P29">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -1704,6 +1882,12 @@
       <c r="N30">
         <v>1e-005</v>
       </c>
+      <c r="O30">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P30">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -1748,6 +1932,12 @@
       <c r="N31">
         <v>1e-005</v>
       </c>
+      <c r="O31">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P31">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -1792,6 +1982,12 @@
       <c r="N32">
         <v>1e-005</v>
       </c>
+      <c r="O32">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P32">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -1836,6 +2032,12 @@
       <c r="N33">
         <v>1e-005</v>
       </c>
+      <c r="O33">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P33">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -1880,6 +2082,12 @@
       <c r="N34">
         <v>1e-005</v>
       </c>
+      <c r="O34">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P34">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -1924,6 +2132,12 @@
       <c r="N35">
         <v>1e-005</v>
       </c>
+      <c r="O35">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P35">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -1968,6 +2182,12 @@
       <c r="N36">
         <v>1e-005</v>
       </c>
+      <c r="O36">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P36">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -2012,6 +2232,12 @@
       <c r="N37">
         <v>1e-005</v>
       </c>
+      <c r="O37">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P37">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -2056,6 +2282,12 @@
       <c r="N38">
         <v>1e-005</v>
       </c>
+      <c r="O38">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P38">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -2100,6 +2332,12 @@
       <c r="N39">
         <v>1e-005</v>
       </c>
+      <c r="O39">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P39">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -2144,6 +2382,12 @@
       <c r="N40">
         <v>1e-005</v>
       </c>
+      <c r="O40">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P40">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -2188,6 +2432,12 @@
       <c r="N41">
         <v>1e-005</v>
       </c>
+      <c r="O41">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P41">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -2232,6 +2482,12 @@
       <c r="N42">
         <v>1e-005</v>
       </c>
+      <c r="O42">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P42">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -2276,6 +2532,12 @@
       <c r="N43">
         <v>1e-005</v>
       </c>
+      <c r="O43">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P43">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -2320,6 +2582,12 @@
       <c r="N44">
         <v>1e-005</v>
       </c>
+      <c r="O44">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P44">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -2364,6 +2632,12 @@
       <c r="N45">
         <v>1e-005</v>
       </c>
+      <c r="O45">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P45">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -2408,6 +2682,12 @@
       <c r="N46">
         <v>1e-005</v>
       </c>
+      <c r="O46">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P46">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -2452,6 +2732,12 @@
       <c r="N47">
         <v>1e-005</v>
       </c>
+      <c r="O47">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P47">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -2496,6 +2782,12 @@
       <c r="N48">
         <v>1e-005</v>
       </c>
+      <c r="O48">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P48">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -2540,6 +2832,12 @@
       <c r="N49">
         <v>1e-005</v>
       </c>
+      <c r="O49">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P49">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -2584,6 +2882,12 @@
       <c r="N50">
         <v>1e-005</v>
       </c>
+      <c r="O50">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P50">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -2628,6 +2932,12 @@
       <c r="N51">
         <v>1e-005</v>
       </c>
+      <c r="O51">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P51">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -2672,6 +2982,12 @@
       <c r="N52">
         <v>1e-005</v>
       </c>
+      <c r="O52">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P52">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -2716,6 +3032,12 @@
       <c r="N53">
         <v>1e-005</v>
       </c>
+      <c r="O53">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P53">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -2760,6 +3082,12 @@
       <c r="N54">
         <v>1e-005</v>
       </c>
+      <c r="O54">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P54">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -2804,6 +3132,12 @@
       <c r="N55">
         <v>1e-005</v>
       </c>
+      <c r="O55">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P55">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -2848,6 +3182,12 @@
       <c r="N56">
         <v>1e-005</v>
       </c>
+      <c r="O56">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P56">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -2892,6 +3232,12 @@
       <c r="N57">
         <v>1e-005</v>
       </c>
+      <c r="O57">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P57">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -2936,6 +3282,12 @@
       <c r="N58">
         <v>1e-005</v>
       </c>
+      <c r="O58">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P58">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -2980,6 +3332,12 @@
       <c r="N59">
         <v>1e-005</v>
       </c>
+      <c r="O59">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P59">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -3024,6 +3382,12 @@
       <c r="N60">
         <v>1e-005</v>
       </c>
+      <c r="O60">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P60">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -3068,6 +3432,12 @@
       <c r="N61">
         <v>1e-005</v>
       </c>
+      <c r="O61">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P61">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -3112,6 +3482,12 @@
       <c r="N62">
         <v>1e-005</v>
       </c>
+      <c r="O62">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P62">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -3156,6 +3532,12 @@
       <c r="N63">
         <v>1e-005</v>
       </c>
+      <c r="O63">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P63">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -3200,6 +3582,12 @@
       <c r="N64">
         <v>1e-005</v>
       </c>
+      <c r="O64">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P64">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -3244,6 +3632,12 @@
       <c r="N65">
         <v>1e-005</v>
       </c>
+      <c r="O65">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P65">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -3288,6 +3682,12 @@
       <c r="N66">
         <v>1e-005</v>
       </c>
+      <c r="O66">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P66">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -3332,6 +3732,12 @@
       <c r="N67">
         <v>1e-005</v>
       </c>
+      <c r="O67">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P67">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -3376,6 +3782,12 @@
       <c r="N68">
         <v>1e-005</v>
       </c>
+      <c r="O68">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P68">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -3420,6 +3832,12 @@
       <c r="N69">
         <v>1e-005</v>
       </c>
+      <c r="O69">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P69">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -3464,6 +3882,12 @@
       <c r="N70">
         <v>1e-005</v>
       </c>
+      <c r="O70">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P70">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -3508,6 +3932,12 @@
       <c r="N71">
         <v>1e-005</v>
       </c>
+      <c r="O71">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P71">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -3552,6 +3982,12 @@
       <c r="N72">
         <v>1e-005</v>
       </c>
+      <c r="O72">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P72">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -3596,6 +4032,12 @@
       <c r="N73">
         <v>1e-005</v>
       </c>
+      <c r="O73">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P73">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -3640,6 +4082,12 @@
       <c r="N74">
         <v>1e-005</v>
       </c>
+      <c r="O74">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P74">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -3684,6 +4132,12 @@
       <c r="N75">
         <v>1e-005</v>
       </c>
+      <c r="O75">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P75">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -3728,6 +4182,12 @@
       <c r="N76">
         <v>1e-005</v>
       </c>
+      <c r="O76">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P76">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -3772,6 +4232,12 @@
       <c r="N77">
         <v>1e-005</v>
       </c>
+      <c r="O77">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P77">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -3816,6 +4282,12 @@
       <c r="N78">
         <v>1e-005</v>
       </c>
+      <c r="O78">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P78">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -3860,6 +4332,12 @@
       <c r="N79">
         <v>1e-005</v>
       </c>
+      <c r="O79">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P79">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -3904,6 +4382,12 @@
       <c r="N80">
         <v>1e-005</v>
       </c>
+      <c r="O80">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P80">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -3948,6 +4432,12 @@
       <c r="N81">
         <v>1e-005</v>
       </c>
+      <c r="O81">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P81">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -3992,6 +4482,12 @@
       <c r="N82">
         <v>1e-005</v>
       </c>
+      <c r="O82">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P82">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -4036,6 +4532,12 @@
       <c r="N83">
         <v>1e-005</v>
       </c>
+      <c r="O83">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P83">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -4080,6 +4582,12 @@
       <c r="N84">
         <v>1e-005</v>
       </c>
+      <c r="O84">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P84">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -4124,6 +4632,12 @@
       <c r="N85">
         <v>1e-005</v>
       </c>
+      <c r="O85">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P85">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -4168,6 +4682,12 @@
       <c r="N86">
         <v>1e-005</v>
       </c>
+      <c r="O86">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P86">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -4212,6 +4732,12 @@
       <c r="N87">
         <v>1e-005</v>
       </c>
+      <c r="O87">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P87">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -4256,6 +4782,12 @@
       <c r="N88">
         <v>1e-005</v>
       </c>
+      <c r="O88">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P88">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -4300,6 +4832,12 @@
       <c r="N89">
         <v>1e-005</v>
       </c>
+      <c r="O89">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P89">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -4344,6 +4882,12 @@
       <c r="N90">
         <v>1e-005</v>
       </c>
+      <c r="O90">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P90">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -4388,6 +4932,12 @@
       <c r="N91">
         <v>1e-005</v>
       </c>
+      <c r="O91">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P91">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -4432,6 +4982,12 @@
       <c r="N92">
         <v>1e-005</v>
       </c>
+      <c r="O92">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P92">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -4476,6 +5032,12 @@
       <c r="N93">
         <v>1e-005</v>
       </c>
+      <c r="O93">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P93">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -4520,6 +5082,12 @@
       <c r="N94">
         <v>1e-005</v>
       </c>
+      <c r="O94">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P94">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -4564,6 +5132,12 @@
       <c r="N95">
         <v>1e-005</v>
       </c>
+      <c r="O95">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P95">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -4608,6 +5182,12 @@
       <c r="N96">
         <v>1e-005</v>
       </c>
+      <c r="O96">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P96">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -4652,6 +5232,12 @@
       <c r="N97">
         <v>1e-005</v>
       </c>
+      <c r="O97">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P97">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -4696,6 +5282,12 @@
       <c r="N98">
         <v>1e-005</v>
       </c>
+      <c r="O98">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P98">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -4740,6 +5332,12 @@
       <c r="N99">
         <v>1e-005</v>
       </c>
+      <c r="O99">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P99">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -4784,6 +5382,12 @@
       <c r="N100">
         <v>1e-005</v>
       </c>
+      <c r="O100">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P100">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -4828,6 +5432,12 @@
       <c r="N101">
         <v>1e-005</v>
       </c>
+      <c r="O101">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P101">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -4872,6 +5482,12 @@
       <c r="N102">
         <v>1e-005</v>
       </c>
+      <c r="O102">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P102">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -4916,6 +5532,12 @@
       <c r="N103">
         <v>1e-005</v>
       </c>
+      <c r="O103">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P103">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -4960,6 +5582,12 @@
       <c r="N104">
         <v>1e-005</v>
       </c>
+      <c r="O104">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P104">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -5004,6 +5632,12 @@
       <c r="N105">
         <v>1e-005</v>
       </c>
+      <c r="O105">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P105">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -5048,6 +5682,12 @@
       <c r="N106">
         <v>1e-005</v>
       </c>
+      <c r="O106">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P106">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -5092,6 +5732,12 @@
       <c r="N107">
         <v>1e-005</v>
       </c>
+      <c r="O107">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P107">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -5136,6 +5782,12 @@
       <c r="N108">
         <v>1e-005</v>
       </c>
+      <c r="O108">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P108">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -5180,6 +5832,12 @@
       <c r="N109">
         <v>1e-005</v>
       </c>
+      <c r="O109">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P109">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -5224,6 +5882,12 @@
       <c r="N110">
         <v>1e-005</v>
       </c>
+      <c r="O110">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P110">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -5268,6 +5932,12 @@
       <c r="N111">
         <v>1e-005</v>
       </c>
+      <c r="O111">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P111">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -5312,6 +5982,12 @@
       <c r="N112">
         <v>1e-005</v>
       </c>
+      <c r="O112">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P112">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -5356,6 +6032,12 @@
       <c r="N113">
         <v>1e-005</v>
       </c>
+      <c r="O113">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P113">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -5400,6 +6082,12 @@
       <c r="N114">
         <v>1e-005</v>
       </c>
+      <c r="O114">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P114">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -5444,6 +6132,12 @@
       <c r="N115">
         <v>1e-005</v>
       </c>
+      <c r="O115">
+        <v>0.0389279048890106</v>
+      </c>
+      <c r="P115">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -5488,6 +6182,12 @@
       <c r="N116">
         <v>0.0009</v>
       </c>
+      <c r="O116">
+        <v>0.06951441117952585</v>
+      </c>
+      <c r="P116">
+        <v>0.06951441117952585</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -5532,6 +6232,12 @@
       <c r="N117">
         <v>0.0031</v>
       </c>
+      <c r="O117">
+        <v>0.07053784189707389</v>
+      </c>
+      <c r="P117">
+        <v>0.07053784189707389</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -5576,6 +6282,12 @@
       <c r="N118">
         <v>0.0055</v>
       </c>
+      <c r="O118">
+        <v>0.07167127340230478</v>
+      </c>
+      <c r="P118">
+        <v>0.07167127340230478</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -5620,6 +6332,12 @@
       <c r="N119">
         <v>0.0074</v>
       </c>
+      <c r="O119">
+        <v>0.07258119877484344</v>
+      </c>
+      <c r="P119">
+        <v>0.07258119877484344</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -5664,6 +6382,12 @@
       <c r="N120">
         <v>0.0106</v>
       </c>
+      <c r="O120">
+        <v>0.0741390899356314</v>
+      </c>
+      <c r="P120">
+        <v>0.0741390899356314</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -5708,6 +6432,12 @@
       <c r="N121">
         <v>0.0146</v>
       </c>
+      <c r="O121">
+        <v>0.07613159652805017</v>
+      </c>
+      <c r="P121">
+        <v>0.07613159652805017</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122">
@@ -5752,6 +6482,12 @@
       <c r="N122">
         <v>0.0189</v>
       </c>
+      <c r="O122">
+        <v>0.07833000743023724</v>
+      </c>
+      <c r="P122">
+        <v>0.07833000743023724</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123">
@@ -5796,6 +6532,12 @@
       <c r="N123">
         <v>0.0214</v>
       </c>
+      <c r="O123">
+        <v>0.07963527603365918</v>
+      </c>
+      <c r="P123">
+        <v>0.07963527603365918</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124">
@@ -5840,6 +6582,12 @@
       <c r="N124">
         <v>0.0244</v>
       </c>
+      <c r="O124">
+        <v>0.08122811582134887</v>
+      </c>
+      <c r="P124">
+        <v>0.08122811582134887</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125">
@@ -5884,6 +6632,12 @@
       <c r="N125">
         <v>0.0279</v>
       </c>
+      <c r="O125">
+        <v>0.08312322584657687</v>
+      </c>
+      <c r="P125">
+        <v>0.08312322584657687</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126">
@@ -5928,6 +6682,12 @@
       <c r="N126">
         <v>0.0317</v>
       </c>
+      <c r="O126">
+        <v>0.08522595785576992</v>
+      </c>
+      <c r="P126">
+        <v>0.08522595785576992</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127">
@@ -5972,6 +6732,12 @@
       <c r="N127">
         <v>0.0346</v>
       </c>
+      <c r="O127">
+        <v>0.08686253321775667</v>
+      </c>
+      <c r="P127">
+        <v>0.08686253321775667</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128">
@@ -6016,6 +6782,12 @@
       <c r="N128">
         <v>0.03630000000000001</v>
       </c>
+      <c r="O128">
+        <v>0.08783479435425165</v>
+      </c>
+      <c r="P128">
+        <v>0.08783479435425165</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129">
@@ -6060,6 +6832,12 @@
       <c r="N129">
         <v>0.0409</v>
       </c>
+      <c r="O129">
+        <v>0.0905136457550601</v>
+      </c>
+      <c r="P129">
+        <v>0.0905136457550601</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130">
@@ -6104,6 +6882,12 @@
       <c r="N130">
         <v>0.0506</v>
       </c>
+      <c r="O130">
+        <v>0.09639442896482363</v>
+      </c>
+      <c r="P130">
+        <v>0.09639442896482363</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131">
@@ -6148,6 +6932,12 @@
       <c r="N131">
         <v>0.06440000000000001</v>
       </c>
+      <c r="O131">
+        <v>0.1053104208747103</v>
+      </c>
+      <c r="P131">
+        <v>0.1053104208747103</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132">
@@ -6192,6 +6982,12 @@
       <c r="N132">
         <v>0.0766</v>
       </c>
+      <c r="O132">
+        <v>0.113737607666449</v>
+      </c>
+      <c r="P132">
+        <v>0.113737607666449</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133">
@@ -6236,6 +7032,12 @@
       <c r="N133">
         <v>0.0883</v>
       </c>
+      <c r="O133">
+        <v>0.1223048612499805</v>
+      </c>
+      <c r="P133">
+        <v>0.1223048612499805</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134">
@@ -6280,6 +7082,12 @@
       <c r="N134">
         <v>0.09870000000000001</v>
       </c>
+      <c r="O134">
+        <v>0.1303215291904085</v>
+      </c>
+      <c r="P134">
+        <v>0.1303215291904085</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135">
@@ -6324,6 +7132,12 @@
       <c r="N135">
         <v>0.1075</v>
       </c>
+      <c r="O135">
+        <v>0.1374005571324786</v>
+      </c>
+      <c r="P135">
+        <v>0.1374005571324786</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136">
@@ -6368,6 +7182,12 @@
       <c r="N136">
         <v>0.1149</v>
       </c>
+      <c r="O136">
+        <v>0.1435631078858985</v>
+      </c>
+      <c r="P136">
+        <v>0.1435631078858985</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -6412,6 +7232,12 @@
       <c r="N137">
         <v>0.1213</v>
       </c>
+      <c r="O137">
+        <v>0.1490471006774894</v>
+      </c>
+      <c r="P137">
+        <v>0.1490471006774894</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138">
@@ -6456,6 +7282,12 @@
       <c r="N138">
         <v>0.1303</v>
       </c>
+      <c r="O138">
+        <v>0.1570001242868304</v>
+      </c>
+      <c r="P138">
+        <v>0.1570001242868304</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139">
@@ -6500,6 +7332,12 @@
       <c r="N139">
         <v>0.1377</v>
       </c>
+      <c r="O139">
+        <v>0.1637493703600535</v>
+      </c>
+      <c r="P139">
+        <v>0.1637493703600535</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140">
@@ -6544,6 +7382,12 @@
       <c r="N140">
         <v>0.1458</v>
       </c>
+      <c r="O140">
+        <v>0.1713528602236799</v>
+      </c>
+      <c r="P140">
+        <v>0.1713528602236799</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141">
@@ -6588,6 +7432,12 @@
       <c r="N141">
         <v>0.1531</v>
       </c>
+      <c r="O141">
+        <v>0.1783970321063801</v>
+      </c>
+      <c r="P141">
+        <v>0.1783970321063801</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142">
@@ -6632,6 +7482,12 @@
       <c r="N142">
         <v>0.1612</v>
       </c>
+      <c r="O142">
+        <v>0.1864236687295442</v>
+      </c>
+      <c r="P142">
+        <v>0.1864236687295442</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143">
@@ -6676,6 +7532,12 @@
       <c r="N143">
         <v>0.1706</v>
       </c>
+      <c r="O143">
+        <v>0.1960126677697039</v>
+      </c>
+      <c r="P143">
+        <v>0.1960126677697039</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144">
@@ -6720,6 +7582,12 @@
       <c r="N144">
         <v>0.1776</v>
       </c>
+      <c r="O144">
+        <v>0.203342032288394</v>
+      </c>
+      <c r="P144">
+        <v>0.203342032288394</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -6764,6 +7632,12 @@
       <c r="N145">
         <v>0.1862</v>
       </c>
+      <c r="O145">
+        <v>0.2125635312766463</v>
+      </c>
+      <c r="P145">
+        <v>0.2125635312766463</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146">
@@ -6808,6 +7682,12 @@
       <c r="N146">
         <v>0.1931</v>
       </c>
+      <c r="O146">
+        <v>0.2201322326012811</v>
+      </c>
+      <c r="P146">
+        <v>0.2201322326012811</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147">
@@ -6852,6 +7732,12 @@
       <c r="N147">
         <v>0.2007</v>
       </c>
+      <c r="O147">
+        <v>0.2286407861736074</v>
+      </c>
+      <c r="P147">
+        <v>0.2286407861736074</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148">
@@ -6896,6 +7782,12 @@
       <c r="N148">
         <v>0.2081</v>
       </c>
+      <c r="O148">
+        <v>0.2370954067999131</v>
+      </c>
+      <c r="P148">
+        <v>0.2370954067999131</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149">
@@ -6940,6 +7832,12 @@
       <c r="N149">
         <v>0.2154</v>
       </c>
+      <c r="O149">
+        <v>0.2455966707084053</v>
+      </c>
+      <c r="P149">
+        <v>0.2455966707084053</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150">
@@ -6984,6 +7882,12 @@
       <c r="N150">
         <v>0.2256</v>
       </c>
+      <c r="O150">
+        <v>0.2577360242627421</v>
+      </c>
+      <c r="P150">
+        <v>0.2577360242627421</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151">
@@ -7028,6 +7932,12 @@
       <c r="N151">
         <v>0.235</v>
       </c>
+      <c r="O151">
+        <v>0.2691845728178585</v>
+      </c>
+      <c r="P151">
+        <v>0.2691845728178585</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152">
@@ -7072,6 +7982,12 @@
       <c r="N152">
         <v>0.2495</v>
       </c>
+      <c r="O152">
+        <v>0.2873159440887026</v>
+      </c>
+      <c r="P152">
+        <v>0.2873159440887026</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153">
@@ -7116,6 +8032,12 @@
       <c r="N153">
         <v>0.2612</v>
       </c>
+      <c r="O153">
+        <v>0.3023434011906068</v>
+      </c>
+      <c r="P153">
+        <v>0.3023434011906068</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154">
@@ -7160,6 +8082,12 @@
       <c r="N154">
         <v>0.2714</v>
       </c>
+      <c r="O154">
+        <v>0.315718456771861</v>
+      </c>
+      <c r="P154">
+        <v>0.315718456771861</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155">
@@ -7204,6 +8132,12 @@
       <c r="N155">
         <v>0.282</v>
       </c>
+      <c r="O155">
+        <v>0.3298745893822011</v>
+      </c>
+      <c r="P155">
+        <v>0.3298745893822011</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156">
@@ -7248,6 +8182,12 @@
       <c r="N156">
         <v>0.2929</v>
       </c>
+      <c r="O156">
+        <v>0.3446890272777161</v>
+      </c>
+      <c r="P156">
+        <v>0.3446890272777161</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157">
@@ -7292,6 +8232,12 @@
       <c r="N157">
         <v>0.3063</v>
       </c>
+      <c r="O157">
+        <v>0.3632356564986821</v>
+      </c>
+      <c r="P157">
+        <v>0.3632356564986821</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158">
@@ -7336,6 +8282,12 @@
       <c r="N158">
         <v>0.3221000000000001</v>
       </c>
+      <c r="O158">
+        <v>0.3855385013162777</v>
+      </c>
+      <c r="P158">
+        <v>0.3855385013162777</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159">
@@ -7380,6 +8332,12 @@
       <c r="N159">
         <v>0.3381</v>
       </c>
+      <c r="O159">
+        <v>0.4085529631331808</v>
+      </c>
+      <c r="P159">
+        <v>0.4085529631331808</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160">
@@ -7424,6 +8382,12 @@
       <c r="N160">
         <v>0.3528</v>
       </c>
+      <c r="O160">
+        <v>0.4300323026240998</v>
+      </c>
+      <c r="P160">
+        <v>0.4300323026240998</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161">
@@ -7468,6 +8432,12 @@
       <c r="N161">
         <v>0.3679</v>
       </c>
+      <c r="O161">
+        <v>0.452384590300082</v>
+      </c>
+      <c r="P161">
+        <v>0.452384590300082</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162">
@@ -7512,6 +8482,12 @@
       <c r="N162">
         <v>0.3833</v>
       </c>
+      <c r="O162">
+        <v>0.4754354846690361</v>
+      </c>
+      <c r="P162">
+        <v>0.4754354846690361</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163">
@@ -7556,6 +8532,12 @@
       <c r="N163">
         <v>0.3999</v>
       </c>
+      <c r="O163">
+        <v>0.5005160041274586</v>
+      </c>
+      <c r="P163">
+        <v>0.5005160041274586</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164">
@@ -7600,6 +8582,12 @@
       <c r="N164">
         <v>0.4133</v>
       </c>
+      <c r="O164">
+        <v>0.5208993188655754</v>
+      </c>
+      <c r="P164">
+        <v>0.5208993188655754</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165">
@@ -7644,6 +8632,12 @@
       <c r="N165">
         <v>0.4259</v>
       </c>
+      <c r="O165">
+        <v>0.5401485608035236</v>
+      </c>
+      <c r="P165">
+        <v>0.5401485608035236</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166">
@@ -7688,6 +8682,12 @@
       <c r="N166">
         <v>0.4398</v>
       </c>
+      <c r="O166">
+        <v>0.5614468833072422</v>
+      </c>
+      <c r="P166">
+        <v>0.5614468833072422</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167">
@@ -7732,6 +8732,12 @@
       <c r="N167">
         <v>0.4518</v>
       </c>
+      <c r="O167">
+        <v>0.5798632603947215</v>
+      </c>
+      <c r="P167">
+        <v>0.5798632603947215</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168">
@@ -7776,6 +8782,12 @@
       <c r="N168">
         <v>0.4643000000000001</v>
       </c>
+      <c r="O168">
+        <v>0.5990531331811108</v>
+      </c>
+      <c r="P168">
+        <v>0.5990531331811108</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169">
@@ -7820,6 +8832,12 @@
       <c r="N169">
         <v>0.4777</v>
       </c>
+      <c r="O169">
+        <v>0.6196070389636222</v>
+      </c>
+      <c r="P169">
+        <v>0.6196070389636222</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170">
@@ -7864,6 +8882,12 @@
       <c r="N170">
         <v>0.4974</v>
       </c>
+      <c r="O170">
+        <v>0.6497378992322245</v>
+      </c>
+      <c r="P170">
+        <v>0.6497378992322245</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -7908,6 +8932,12 @@
       <c r="N171">
         <v>0.5177999999999999</v>
       </c>
+      <c r="O171">
+        <v>0.6807566143770127</v>
+      </c>
+      <c r="P171">
+        <v>0.6807566143770127</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172">
@@ -7952,6 +8982,12 @@
       <c r="N172">
         <v>0.5366000000000001</v>
       </c>
+      <c r="O172">
+        <v>0.7091088080089234</v>
+      </c>
+      <c r="P172">
+        <v>0.7091088080089234</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173">
@@ -7996,6 +9032,12 @@
       <c r="N173">
         <v>0.5523</v>
       </c>
+      <c r="O173">
+        <v>0.7325703208070622</v>
+      </c>
+      <c r="P173">
+        <v>0.7325703208070622</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174">
@@ -8040,6 +9082,12 @@
       <c r="N174">
         <v>0.5671000000000001</v>
       </c>
+      <c r="O174">
+        <v>0.7544768952050482</v>
+      </c>
+      <c r="P174">
+        <v>0.7544768952050482</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175">
@@ -8084,6 +9132,12 @@
       <c r="N175">
         <v>0.5816</v>
       </c>
+      <c r="O175">
+        <v>0.7757176360900322</v>
+      </c>
+      <c r="P175">
+        <v>0.7757176360900322</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176">
@@ -8128,6 +9182,12 @@
       <c r="N176">
         <v>0.5972000000000001</v>
       </c>
+      <c r="O176">
+        <v>0.7983000580427608</v>
+      </c>
+      <c r="P176">
+        <v>0.7983000580427608</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177">
@@ -8172,6 +9232,12 @@
       <c r="N177">
         <v>0.6116</v>
       </c>
+      <c r="O177">
+        <v>0.8188766615268707</v>
+      </c>
+      <c r="P177">
+        <v>0.8188766615268707</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178">
@@ -8216,6 +9282,12 @@
       <c r="N178">
         <v>0.6265000000000001</v>
       </c>
+      <c r="O178">
+        <v>0.8398769927609858</v>
+      </c>
+      <c r="P178">
+        <v>0.8398769927609858</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179">
@@ -8260,6 +9332,12 @@
       <c r="N179">
         <v>0.6406000000000001</v>
       </c>
+      <c r="O179">
+        <v>0.8594617091077892</v>
+      </c>
+      <c r="P179">
+        <v>0.8594617091077892</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180">
@@ -8304,6 +9382,12 @@
       <c r="N180">
         <v>0.6563</v>
       </c>
+      <c r="O180">
+        <v>0.8809224428037336</v>
+      </c>
+      <c r="P180">
+        <v>0.8809224428037336</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181">
@@ -8348,6 +9432,12 @@
       <c r="N181">
         <v>0.6727000000000001</v>
       </c>
+      <c r="O181">
+        <v>0.9029329714524594</v>
+      </c>
+      <c r="P181">
+        <v>0.9029329714524594</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182">
@@ -8392,6 +9482,12 @@
       <c r="N182">
         <v>0.6882</v>
       </c>
+      <c r="O182">
+        <v>0.9233385479323967</v>
+      </c>
+      <c r="P182">
+        <v>0.9233385479323967</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183">
@@ -8436,6 +9532,12 @@
       <c r="N183">
         <v>0.7018</v>
       </c>
+      <c r="O183">
+        <v>0.9409151890106349</v>
+      </c>
+      <c r="P183">
+        <v>0.9409151890106349</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184">
@@ -8480,6 +9582,12 @@
       <c r="N184">
         <v>0.7171000000000001</v>
       </c>
+      <c r="O184">
+        <v>0.9603137309529012</v>
+      </c>
+      <c r="P184">
+        <v>0.9603137309529012</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185">
@@ -8524,6 +9632,12 @@
       <c r="N185">
         <v>0.734</v>
       </c>
+      <c r="O185">
+        <v>0.9812693857627449</v>
+      </c>
+      <c r="P185">
+        <v>0.9812693857627449</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186">
@@ -8568,6 +9682,12 @@
       <c r="N186">
         <v>0.7509</v>
       </c>
+      <c r="O186">
+        <v>1.001721170052791</v>
+      </c>
+      <c r="P186">
+        <v>1.001721170052791</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187">
@@ -8612,6 +9732,12 @@
       <c r="N187">
         <v>0.7675000000000001</v>
       </c>
+      <c r="O187">
+        <v>1.021312434007042</v>
+      </c>
+      <c r="P187">
+        <v>1.021312434007042</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188">
@@ -8656,6 +9782,12 @@
       <c r="N188">
         <v>0.7839</v>
       </c>
+      <c r="O188">
+        <v>1.040178672064331</v>
+      </c>
+      <c r="P188">
+        <v>1.040178672064331</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189">
@@ -8700,6 +9832,12 @@
       <c r="N189">
         <v>0.7994</v>
       </c>
+      <c r="O189">
+        <v>1.057560009920631</v>
+      </c>
+      <c r="P189">
+        <v>1.057560009920631</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190">
@@ -8744,6 +9882,12 @@
       <c r="N190">
         <v>0.8147000000000001</v>
       </c>
+      <c r="O190">
+        <v>1.074287263851218</v>
+      </c>
+      <c r="P190">
+        <v>1.074287263851218</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191">
@@ -8788,6 +9932,12 @@
       <c r="N191">
         <v>0.8292999999999999</v>
       </c>
+      <c r="O191">
+        <v>1.089850856679496</v>
+      </c>
+      <c r="P191">
+        <v>1.089850856679496</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192">
@@ -8832,6 +9982,12 @@
       <c r="N192">
         <v>0.844</v>
       </c>
+      <c r="O192">
+        <v>1.105128686571407</v>
+      </c>
+      <c r="P192">
+        <v>1.105128686571407</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193">
@@ -8876,6 +10032,12 @@
       <c r="N193">
         <v>0.859</v>
       </c>
+      <c r="O193">
+        <v>1.12031399305816</v>
+      </c>
+      <c r="P193">
+        <v>1.12031399305816</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194">
@@ -8920,6 +10082,12 @@
       <c r="N194">
         <v>0.8748</v>
       </c>
+      <c r="O194">
+        <v>1.135870090595415</v>
+      </c>
+      <c r="P194">
+        <v>1.135870090595415</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195">
@@ -8964,6 +10132,12 @@
       <c r="N195">
         <v>0.8915000000000001</v>
       </c>
+      <c r="O195">
+        <v>1.151826497600368</v>
+      </c>
+      <c r="P195">
+        <v>1.151826497600368</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196">
@@ -9008,6 +10182,12 @@
       <c r="N196">
         <v>0.91</v>
       </c>
+      <c r="O196">
+        <v>1.168926104919557</v>
+      </c>
+      <c r="P196">
+        <v>1.168926104919557</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197">
@@ -9052,6 +10232,12 @@
       <c r="N197">
         <v>0.9295</v>
       </c>
+      <c r="O197">
+        <v>1.186302782534555</v>
+      </c>
+      <c r="P197">
+        <v>1.186302782534555</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198">
@@ -9096,6 +10282,12 @@
       <c r="N198">
         <v>0.9492</v>
       </c>
+      <c r="O198">
+        <v>1.203194372116121</v>
+      </c>
+      <c r="P198">
+        <v>1.203194372116121</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199">
@@ -9140,6 +10332,12 @@
       <c r="N199">
         <v>0.9682999999999999</v>
       </c>
+      <c r="O199">
+        <v>1.218947021130129</v>
+      </c>
+      <c r="P199">
+        <v>1.218947021130129</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200">
@@ -9184,6 +10382,12 @@
       <c r="N200">
         <v>0.9841000000000001</v>
       </c>
+      <c r="O200">
+        <v>1.231522455203165</v>
+      </c>
+      <c r="P200">
+        <v>1.231522455203165</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201">
@@ -9228,6 +10432,12 @@
       <c r="N201">
         <v>0.99</v>
       </c>
+      <c r="O201">
+        <v>1.243314493836145</v>
+      </c>
+      <c r="P201">
+        <v>1.243314493836145</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202">
@@ -9272,6 +10482,12 @@
       <c r="N202">
         <v>0.99</v>
       </c>
+      <c r="O202">
+        <v>1.254367178690707</v>
+      </c>
+      <c r="P202">
+        <v>1.254367178690707</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203">
@@ -9316,6 +10532,12 @@
       <c r="N203">
         <v>0.99</v>
       </c>
+      <c r="O203">
+        <v>1.26543457055257</v>
+      </c>
+      <c r="P203">
+        <v>1.26543457055257</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -9360,6 +10582,12 @@
       <c r="N204">
         <v>0.99</v>
       </c>
+      <c r="O204">
+        <v>1.276144891425343</v>
+      </c>
+      <c r="P204">
+        <v>1.276144891425343</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205">
@@ -9404,6 +10632,12 @@
       <c r="N205">
         <v>0.99</v>
       </c>
+      <c r="O205">
+        <v>1.287038272318417</v>
+      </c>
+      <c r="P205">
+        <v>1.287038272318417</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206">
@@ -9448,6 +10682,12 @@
       <c r="N206">
         <v>0.99</v>
       </c>
+      <c r="O206">
+        <v>1.297425871280462</v>
+      </c>
+      <c r="P206">
+        <v>1.297425871280462</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207">
@@ -9492,6 +10732,12 @@
       <c r="N207">
         <v>0.99</v>
       </c>
+      <c r="O207">
+        <v>1.30739245520153</v>
+      </c>
+      <c r="P207">
+        <v>1.30739245520153</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208">
@@ -9536,6 +10782,12 @@
       <c r="N208">
         <v>0.99</v>
       </c>
+      <c r="O208">
+        <v>1.31784959619977</v>
+      </c>
+      <c r="P208">
+        <v>1.31784959619977</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209">
@@ -9580,6 +10832,12 @@
       <c r="N209">
         <v>0.99</v>
       </c>
+      <c r="O209">
+        <v>1.328309971843823</v>
+      </c>
+      <c r="P209">
+        <v>1.328309971843823</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210">
@@ -9624,6 +10882,12 @@
       <c r="N210">
         <v>0.99</v>
       </c>
+      <c r="O210">
+        <v>1.337416372718857</v>
+      </c>
+      <c r="P210">
+        <v>1.337416372718857</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211">
@@ -9668,6 +10932,12 @@
       <c r="N211">
         <v>0.99</v>
       </c>
+      <c r="O211">
+        <v>1.345071332379754</v>
+      </c>
+      <c r="P211">
+        <v>1.345071332379754</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212">
@@ -9712,6 +10982,12 @@
       <c r="N212">
         <v>0.99</v>
       </c>
+      <c r="O212">
+        <v>1.352842351008244</v>
+      </c>
+      <c r="P212">
+        <v>1.352842351008244</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213">
@@ -9756,6 +11032,12 @@
       <c r="N213">
         <v>0.99</v>
       </c>
+      <c r="O213">
+        <v>1.360000938529711</v>
+      </c>
+      <c r="P213">
+        <v>1.360000938529711</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214">
@@ -9800,6 +11082,12 @@
       <c r="N214">
         <v>0.99</v>
       </c>
+      <c r="O214">
+        <v>1.366636900071521</v>
+      </c>
+      <c r="P214">
+        <v>1.366636900071521</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215">
@@ -9844,6 +11132,12 @@
       <c r="N215">
         <v>0.99</v>
       </c>
+      <c r="O215">
+        <v>1.372455019979125</v>
+      </c>
+      <c r="P215">
+        <v>1.372455019979125</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216">
@@ -9888,6 +11182,12 @@
       <c r="N216">
         <v>0.99</v>
       </c>
+      <c r="O216">
+        <v>1.37806183454179</v>
+      </c>
+      <c r="P216">
+        <v>1.37806183454179</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217">
@@ -9932,6 +11232,12 @@
       <c r="N217">
         <v>0.99</v>
       </c>
+      <c r="O217">
+        <v>1.383819949377734</v>
+      </c>
+      <c r="P217">
+        <v>1.383819949377734</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218">
@@ -9976,6 +11282,12 @@
       <c r="N218">
         <v>0.99</v>
       </c>
+      <c r="O218">
+        <v>1.389060530994368</v>
+      </c>
+      <c r="P218">
+        <v>1.389060530994368</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219">
@@ -10020,6 +11332,12 @@
       <c r="N219">
         <v>0.99</v>
       </c>
+      <c r="O219">
+        <v>1.394152304464184</v>
+      </c>
+      <c r="P219">
+        <v>1.394152304464184</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220">
@@ -10064,6 +11382,12 @@
       <c r="N220">
         <v>0.99</v>
       </c>
+      <c r="O220">
+        <v>1.399707191556029</v>
+      </c>
+      <c r="P220">
+        <v>1.399707191556029</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221">
@@ -10108,6 +11432,12 @@
       <c r="N221">
         <v>0.99</v>
       </c>
+      <c r="O221">
+        <v>1.405474690911378</v>
+      </c>
+      <c r="P221">
+        <v>1.405474690911378</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222">
@@ -10152,6 +11482,12 @@
       <c r="N222">
         <v>0.99</v>
       </c>
+      <c r="O222">
+        <v>1.410740209537468</v>
+      </c>
+      <c r="P222">
+        <v>1.410740209537468</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223">
@@ -10196,6 +11532,12 @@
       <c r="N223">
         <v>0.99</v>
       </c>
+      <c r="O223">
+        <v>1.415576337586701</v>
+      </c>
+      <c r="P223">
+        <v>1.415576337586701</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224">
@@ -10240,6 +11582,12 @@
       <c r="N224">
         <v>0.99</v>
       </c>
+      <c r="O224">
+        <v>1.420508714956663</v>
+      </c>
+      <c r="P224">
+        <v>1.420508714956663</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225">
@@ -10284,6 +11632,12 @@
       <c r="N225">
         <v>0.99</v>
       </c>
+      <c r="O225">
+        <v>1.425755787237473</v>
+      </c>
+      <c r="P225">
+        <v>1.425755787237473</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226">
@@ -10328,6 +11682,12 @@
       <c r="N226">
         <v>0.99</v>
       </c>
+      <c r="O226">
+        <v>1.431564049657638</v>
+      </c>
+      <c r="P226">
+        <v>1.431564049657638</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227">
@@ -10372,6 +11732,12 @@
       <c r="N227">
         <v>0.99</v>
       </c>
+      <c r="O227">
+        <v>1.435963901632616</v>
+      </c>
+      <c r="P227">
+        <v>1.435963901632616</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228">
@@ -10416,6 +11782,12 @@
       <c r="N228">
         <v>0.99</v>
       </c>
+      <c r="O228">
+        <v>1.44033805530067</v>
+      </c>
+      <c r="P228">
+        <v>1.44033805530067</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229">
@@ -10460,6 +11832,12 @@
       <c r="N229">
         <v>0.99</v>
       </c>
+      <c r="O229">
+        <v>1.443911616296841</v>
+      </c>
+      <c r="P229">
+        <v>1.443911616296841</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230">
@@ -10504,6 +11882,12 @@
       <c r="N230">
         <v>0.99</v>
       </c>
+      <c r="O230">
+        <v>1.446862113653845</v>
+      </c>
+      <c r="P230">
+        <v>1.446862113653845</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231">
@@ -10548,6 +11932,12 @@
       <c r="N231">
         <v>0.99</v>
       </c>
+      <c r="O231">
+        <v>1.450299663957279</v>
+      </c>
+      <c r="P231">
+        <v>1.450299663957279</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232">
@@ -10592,6 +11982,12 @@
       <c r="N232">
         <v>0.99</v>
       </c>
+      <c r="O232">
+        <v>1.453769608749467</v>
+      </c>
+      <c r="P232">
+        <v>1.453769608749467</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -10636,6 +12032,12 @@
       <c r="N233">
         <v>0.99</v>
       </c>
+      <c r="O233">
+        <v>1.456946917573664</v>
+      </c>
+      <c r="P233">
+        <v>1.456946917573664</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -10680,6 +12082,12 @@
       <c r="N234">
         <v>0.99</v>
       </c>
+      <c r="O234">
+        <v>1.459953336479944</v>
+      </c>
+      <c r="P234">
+        <v>1.459953336479944</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -10724,6 +12132,12 @@
       <c r="N235">
         <v>0.99</v>
       </c>
+      <c r="O235">
+        <v>1.462499889411433</v>
+      </c>
+      <c r="P235">
+        <v>1.462499889411433</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236">
@@ -10768,6 +12182,12 @@
       <c r="N236">
         <v>0.99</v>
       </c>
+      <c r="O236">
+        <v>1.46493335154758</v>
+      </c>
+      <c r="P236">
+        <v>1.46493335154758</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -10812,6 +12232,12 @@
       <c r="N237">
         <v>0.99</v>
       </c>
+      <c r="O237">
+        <v>1.46751897989872</v>
+      </c>
+      <c r="P237">
+        <v>1.46751897989872</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -10856,6 +12282,12 @@
       <c r="N238">
         <v>0.99</v>
       </c>
+      <c r="O238">
+        <v>1.470423969669185</v>
+      </c>
+      <c r="P238">
+        <v>1.470423969669185</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239">
@@ -10900,6 +12332,12 @@
       <c r="N239">
         <v>0.99</v>
       </c>
+      <c r="O239">
+        <v>1.472570493102155</v>
+      </c>
+      <c r="P239">
+        <v>1.472570493102155</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240">
@@ -10944,6 +12382,12 @@
       <c r="N240">
         <v>0.99</v>
       </c>
+      <c r="O240">
+        <v>1.475121657861295</v>
+      </c>
+      <c r="P240">
+        <v>1.475121657861295</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241">
@@ -10988,6 +12432,12 @@
       <c r="N241">
         <v>0.99</v>
       </c>
+      <c r="O241">
+        <v>1.47753488446847</v>
+      </c>
+      <c r="P241">
+        <v>1.47753488446847</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -11032,6 +12482,12 @@
       <c r="N242">
         <v>0.99</v>
       </c>
+      <c r="O242">
+        <v>1.480266516112227</v>
+      </c>
+      <c r="P242">
+        <v>1.480266516112227</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243">
@@ -11076,6 +12532,12 @@
       <c r="N243">
         <v>0.99</v>
       </c>
+      <c r="O243">
+        <v>1.482847822638183</v>
+      </c>
+      <c r="P243">
+        <v>1.482847822638183</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244">
@@ -11120,6 +12582,12 @@
       <c r="N244">
         <v>0.99</v>
       </c>
+      <c r="O244">
+        <v>1.485401698279428</v>
+      </c>
+      <c r="P244">
+        <v>1.485401698279428</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245">
@@ -11164,6 +12632,12 @@
       <c r="N245">
         <v>0.99</v>
       </c>
+      <c r="O245">
+        <v>1.487777930795272</v>
+      </c>
+      <c r="P245">
+        <v>1.487777930795272</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246">
@@ -11208,6 +12682,12 @@
       <c r="N246">
         <v>0.99</v>
       </c>
+      <c r="O246">
+        <v>1.490272902489446</v>
+      </c>
+      <c r="P246">
+        <v>1.490272902489446</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247">
@@ -11252,6 +12732,12 @@
       <c r="N247">
         <v>0.99</v>
       </c>
+      <c r="O247">
+        <v>1.492680134474413</v>
+      </c>
+      <c r="P247">
+        <v>1.492680134474413</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248">
@@ -11296,6 +12782,12 @@
       <c r="N248">
         <v>0.99</v>
       </c>
+      <c r="O248">
+        <v>1.494337958282061</v>
+      </c>
+      <c r="P248">
+        <v>1.494337958282061</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249">
@@ -11340,6 +12832,12 @@
       <c r="N249">
         <v>0.99</v>
       </c>
+      <c r="O249">
+        <v>1.49544728697219</v>
+      </c>
+      <c r="P249">
+        <v>1.49544728697219</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250">
@@ -11384,6 +12882,12 @@
       <c r="N250">
         <v>0.99</v>
       </c>
+      <c r="O250">
+        <v>1.496811021447851</v>
+      </c>
+      <c r="P250">
+        <v>1.496811021447851</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251">
@@ -11428,6 +12932,12 @@
       <c r="N251">
         <v>0.99</v>
       </c>
+      <c r="O251">
+        <v>1.498708138183639</v>
+      </c>
+      <c r="P251">
+        <v>1.498708138183639</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252">
@@ -11472,6 +12982,12 @@
       <c r="N252">
         <v>0.99</v>
       </c>
+      <c r="O252">
+        <v>1.500892632697612</v>
+      </c>
+      <c r="P252">
+        <v>1.500892632697612</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253">
@@ -11516,6 +13032,12 @@
       <c r="N253">
         <v>0.99</v>
       </c>
+      <c r="O253">
+        <v>1.503097988432174</v>
+      </c>
+      <c r="P253">
+        <v>1.503097988432174</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254">
@@ -11560,6 +13082,12 @@
       <c r="N254">
         <v>0.99</v>
       </c>
+      <c r="O254">
+        <v>1.504898676807363</v>
+      </c>
+      <c r="P254">
+        <v>1.504898676807363</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255">
@@ -11604,6 +13132,12 @@
       <c r="N255">
         <v>0.99</v>
       </c>
+      <c r="O255">
+        <v>1.506882609375528</v>
+      </c>
+      <c r="P255">
+        <v>1.506882609375528</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256">
@@ -11648,6 +13182,12 @@
       <c r="N256">
         <v>0.99</v>
       </c>
+      <c r="O256">
+        <v>1.508818293355545</v>
+      </c>
+      <c r="P256">
+        <v>1.508818293355545</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257">
@@ -11692,6 +13232,12 @@
       <c r="N257">
         <v>0.99</v>
       </c>
+      <c r="O257">
+        <v>1.510406464403558</v>
+      </c>
+      <c r="P257">
+        <v>1.510406464403558</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258">
@@ -11736,6 +13282,12 @@
       <c r="N258">
         <v>0.99</v>
       </c>
+      <c r="O258">
+        <v>1.511761496402277</v>
+      </c>
+      <c r="P258">
+        <v>1.511761496402277</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259">
@@ -11780,6 +13332,12 @@
       <c r="N259">
         <v>0.99</v>
       </c>
+      <c r="O259">
+        <v>1.51300701604163</v>
+      </c>
+      <c r="P259">
+        <v>1.51300701604163</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260">
@@ -11824,6 +13382,12 @@
       <c r="N260">
         <v>0.99</v>
       </c>
+      <c r="O260">
+        <v>1.514528070664355</v>
+      </c>
+      <c r="P260">
+        <v>1.514528070664355</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261">
@@ -11868,6 +13432,12 @@
       <c r="N261">
         <v>0.99</v>
       </c>
+      <c r="O261">
+        <v>1.515809621831342</v>
+      </c>
+      <c r="P261">
+        <v>1.515809621831342</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262">
@@ -11912,6 +13482,12 @@
       <c r="N262">
         <v>0.99</v>
       </c>
+      <c r="O262">
+        <v>1.516816090434459</v>
+      </c>
+      <c r="P262">
+        <v>1.516816090434459</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263">
@@ -11956,6 +13532,12 @@
       <c r="N263">
         <v>0.99</v>
       </c>
+      <c r="O263">
+        <v>1.51754443186024</v>
+      </c>
+      <c r="P263">
+        <v>1.51754443186024</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264">
@@ -12000,6 +13582,12 @@
       <c r="N264">
         <v>0.99</v>
       </c>
+      <c r="O264">
+        <v>1.51814494481398</v>
+      </c>
+      <c r="P264">
+        <v>1.51814494481398</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265">
@@ -12044,6 +13632,12 @@
       <c r="N265">
         <v>0.99</v>
       </c>
+      <c r="O265">
+        <v>1.518829057442626</v>
+      </c>
+      <c r="P265">
+        <v>1.518829057442626</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266">
@@ -12088,6 +13682,12 @@
       <c r="N266">
         <v>0.99</v>
       </c>
+      <c r="O266">
+        <v>1.519813055080473</v>
+      </c>
+      <c r="P266">
+        <v>1.519813055080473</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267">
@@ -12132,6 +13732,12 @@
       <c r="N267">
         <v>0.99</v>
       </c>
+      <c r="O267">
+        <v>1.520840358385766</v>
+      </c>
+      <c r="P267">
+        <v>1.520840358385766</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268">
@@ -12176,6 +13782,12 @@
       <c r="N268">
         <v>0.99</v>
       </c>
+      <c r="O268">
+        <v>1.521858684994323</v>
+      </c>
+      <c r="P268">
+        <v>1.521858684994323</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269">
@@ -12220,6 +13832,12 @@
       <c r="N269">
         <v>0.99</v>
       </c>
+      <c r="O269">
+        <v>1.522857993294675</v>
+      </c>
+      <c r="P269">
+        <v>1.522857993294675</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270">
@@ -12264,6 +13882,12 @@
       <c r="N270">
         <v>0.99</v>
       </c>
+      <c r="O270">
+        <v>1.523604842634069</v>
+      </c>
+      <c r="P270">
+        <v>1.523604842634069</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271">
@@ -12308,6 +13932,12 @@
       <c r="N271">
         <v>0.99</v>
       </c>
+      <c r="O271">
+        <v>1.524642705287329</v>
+      </c>
+      <c r="P271">
+        <v>1.524642705287329</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272">
@@ -12352,6 +13982,12 @@
       <c r="N272">
         <v>0.99</v>
       </c>
+      <c r="O272">
+        <v>1.525614918626179</v>
+      </c>
+      <c r="P272">
+        <v>1.525614918626179</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273">
@@ -12396,6 +14032,12 @@
       <c r="N273">
         <v>0.99</v>
       </c>
+      <c r="O273">
+        <v>1.526459510009426</v>
+      </c>
+      <c r="P273">
+        <v>1.526459510009426</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274">
@@ -12440,6 +14082,12 @@
       <c r="N274">
         <v>0.99</v>
       </c>
+      <c r="O274">
+        <v>1.527136793546274</v>
+      </c>
+      <c r="P274">
+        <v>1.527136793546274</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275">
@@ -12484,6 +14132,12 @@
       <c r="N275">
         <v>0.99</v>
       </c>
+      <c r="O275">
+        <v>1.527878113938668</v>
+      </c>
+      <c r="P275">
+        <v>1.527878113938668</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276">
@@ -12528,6 +14182,12 @@
       <c r="N276">
         <v>0.99</v>
       </c>
+      <c r="O276">
+        <v>1.528632006622301</v>
+      </c>
+      <c r="P276">
+        <v>1.528632006622301</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277">
@@ -12572,6 +14232,12 @@
       <c r="N277">
         <v>0.99</v>
       </c>
+      <c r="O277">
+        <v>1.529567803246502</v>
+      </c>
+      <c r="P277">
+        <v>1.529567803246502</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278">
@@ -12616,6 +14282,12 @@
       <c r="N278">
         <v>0.99</v>
       </c>
+      <c r="O278">
+        <v>1.530314718721635</v>
+      </c>
+      <c r="P278">
+        <v>1.530314718721635</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279">
@@ -12660,6 +14332,12 @@
       <c r="N279">
         <v>0.99</v>
       </c>
+      <c r="O279">
+        <v>1.530879409207022</v>
+      </c>
+      <c r="P279">
+        <v>1.530879409207022</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280">
@@ -12704,6 +14382,12 @@
       <c r="N280">
         <v>0.99</v>
       </c>
+      <c r="O280">
+        <v>1.531522195079152</v>
+      </c>
+      <c r="P280">
+        <v>1.531522195079152</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281">
@@ -12748,6 +14432,12 @@
       <c r="N281">
         <v>0.99</v>
       </c>
+      <c r="O281">
+        <v>1.53190579761375</v>
+      </c>
+      <c r="P281">
+        <v>1.53190579761375</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282">
@@ -12792,6 +14482,12 @@
       <c r="N282">
         <v>0.99</v>
       </c>
+      <c r="O282">
+        <v>1.532250194508933</v>
+      </c>
+      <c r="P282">
+        <v>1.532250194508933</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283">
@@ -12836,6 +14532,12 @@
       <c r="N283">
         <v>0.99</v>
       </c>
+      <c r="O283">
+        <v>1.532688977710675</v>
+      </c>
+      <c r="P283">
+        <v>1.532688977710675</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284">
@@ -12880,6 +14582,12 @@
       <c r="N284">
         <v>0.99</v>
       </c>
+      <c r="O284">
+        <v>1.532957685140759</v>
+      </c>
+      <c r="P284">
+        <v>1.532957685140759</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285">
@@ -12924,6 +14632,12 @@
       <c r="N285">
         <v>0.99</v>
       </c>
+      <c r="O285">
+        <v>1.533409705016631</v>
+      </c>
+      <c r="P285">
+        <v>1.533409705016631</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286">
@@ -12968,6 +14682,12 @@
       <c r="N286">
         <v>0.99</v>
       </c>
+      <c r="O286">
+        <v>1.533676885532125</v>
+      </c>
+      <c r="P286">
+        <v>1.533676885532125</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287">
@@ -13012,6 +14732,12 @@
       <c r="N287">
         <v>0.99</v>
       </c>
+      <c r="O287">
+        <v>1.533916049011964</v>
+      </c>
+      <c r="P287">
+        <v>1.533916049011964</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288">
@@ -13056,6 +14782,12 @@
       <c r="N288">
         <v>0.99</v>
       </c>
+      <c r="O288">
+        <v>1.534381010655734</v>
+      </c>
+      <c r="P288">
+        <v>1.534381010655734</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289">
@@ -13100,6 +14832,12 @@
       <c r="N289">
         <v>0.99</v>
       </c>
+      <c r="O289">
+        <v>1.53483072234403</v>
+      </c>
+      <c r="P289">
+        <v>1.53483072234403</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290">
@@ -13144,6 +14882,12 @@
       <c r="N290">
         <v>0.99</v>
       </c>
+      <c r="O290">
+        <v>1.53517702802786</v>
+      </c>
+      <c r="P290">
+        <v>1.53517702802786</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291">
@@ -13188,6 +14932,12 @@
       <c r="N291">
         <v>0.99</v>
       </c>
+      <c r="O291">
+        <v>1.535506330696151</v>
+      </c>
+      <c r="P291">
+        <v>1.535506330696151</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292">
@@ -13232,6 +14982,12 @@
       <c r="N292">
         <v>0.99</v>
       </c>
+      <c r="O292">
+        <v>1.535616941741763</v>
+      </c>
+      <c r="P292">
+        <v>1.535616941741763</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293">
@@ -13276,6 +15032,12 @@
       <c r="N293">
         <v>0.99</v>
       </c>
+      <c r="O293">
+        <v>1.536087914785212</v>
+      </c>
+      <c r="P293">
+        <v>1.536087914785212</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294">
@@ -13320,6 +15082,12 @@
       <c r="N294">
         <v>0.99</v>
       </c>
+      <c r="O294">
+        <v>1.536731245184847</v>
+      </c>
+      <c r="P294">
+        <v>1.536731245184847</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295">
@@ -13364,6 +15132,12 @@
       <c r="N295">
         <v>0.99</v>
       </c>
+      <c r="O295">
+        <v>1.53710242989504</v>
+      </c>
+      <c r="P295">
+        <v>1.53710242989504</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296">
@@ -13408,6 +15182,12 @@
       <c r="N296">
         <v>0.99</v>
       </c>
+      <c r="O296">
+        <v>1.537312283564354</v>
+      </c>
+      <c r="P296">
+        <v>1.537312283564354</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297">
@@ -13452,6 +15232,12 @@
       <c r="N297">
         <v>0.99</v>
       </c>
+      <c r="O297">
+        <v>1.537530546936814</v>
+      </c>
+      <c r="P297">
+        <v>1.537530546936814</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298">
@@ -13496,6 +15282,12 @@
       <c r="N298">
         <v>0.99</v>
       </c>
+      <c r="O298">
+        <v>1.537741187917224</v>
+      </c>
+      <c r="P298">
+        <v>1.537741187917224</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299">
@@ -13540,6 +15332,12 @@
       <c r="N299">
         <v>0.99</v>
       </c>
+      <c r="O299">
+        <v>1.537861287751952</v>
+      </c>
+      <c r="P299">
+        <v>1.537861287751952</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300">
@@ -13584,6 +15382,12 @@
       <c r="N300">
         <v>0.99</v>
       </c>
+      <c r="O300">
+        <v>1.53822739361049</v>
+      </c>
+      <c r="P300">
+        <v>1.53822739361049</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301">
@@ -13628,6 +15432,12 @@
       <c r="N301">
         <v>0.99</v>
       </c>
+      <c r="O301">
+        <v>1.538716432813582</v>
+      </c>
+      <c r="P301">
+        <v>1.538716432813582</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302">
@@ -13672,6 +15482,12 @@
       <c r="N302">
         <v>0.99</v>
       </c>
+      <c r="O302">
+        <v>1.539183212821602</v>
+      </c>
+      <c r="P302">
+        <v>1.539183212821602</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303">
@@ -13716,6 +15532,12 @@
       <c r="N303">
         <v>0.99</v>
       </c>
+      <c r="O303">
+        <v>1.539505334070773</v>
+      </c>
+      <c r="P303">
+        <v>1.539505334070773</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304">
@@ -13760,6 +15582,12 @@
       <c r="N304">
         <v>0.99</v>
       </c>
+      <c r="O304">
+        <v>1.539732572366882</v>
+      </c>
+      <c r="P304">
+        <v>1.539732572366882</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305">
@@ -13804,6 +15632,12 @@
       <c r="N305">
         <v>0.99</v>
       </c>
+      <c r="O305">
+        <v>1.540095646981726</v>
+      </c>
+      <c r="P305">
+        <v>1.540095646981726</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306">
@@ -13848,6 +15682,12 @@
       <c r="N306">
         <v>0.99</v>
       </c>
+      <c r="O306">
+        <v>1.54045119764051</v>
+      </c>
+      <c r="P306">
+        <v>1.54045119764051</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307">
@@ -13892,6 +15732,12 @@
       <c r="N307">
         <v>0.99</v>
       </c>
+      <c r="O307">
+        <v>1.540675228881878</v>
+      </c>
+      <c r="P307">
+        <v>1.540675228881878</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308">
@@ -13936,6 +15782,12 @@
       <c r="N308">
         <v>0.99</v>
       </c>
+      <c r="O308">
+        <v>1.540777277376568</v>
+      </c>
+      <c r="P308">
+        <v>1.540777277376568</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309">
@@ -13980,6 +15832,12 @@
       <c r="N309">
         <v>0.99</v>
       </c>
+      <c r="O309">
+        <v>1.540918213249214</v>
+      </c>
+      <c r="P309">
+        <v>1.540918213249214</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310">
@@ -14024,6 +15882,12 @@
       <c r="N310">
         <v>0.99</v>
       </c>
+      <c r="O310">
+        <v>1.541114365806527</v>
+      </c>
+      <c r="P310">
+        <v>1.541114365806527</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311">
@@ -14068,6 +15932,12 @@
       <c r="N311">
         <v>0.99</v>
       </c>
+      <c r="O311">
+        <v>1.541402056363005</v>
+      </c>
+      <c r="P311">
+        <v>1.541402056363005</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312">
@@ -14112,6 +15982,12 @@
       <c r="N312">
         <v>0.99</v>
       </c>
+      <c r="O312">
+        <v>1.541646953596073</v>
+      </c>
+      <c r="P312">
+        <v>1.541646953596073</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313">
@@ -14156,6 +16032,12 @@
       <c r="N313">
         <v>0.99</v>
       </c>
+      <c r="O313">
+        <v>1.541718013421261</v>
+      </c>
+      <c r="P313">
+        <v>1.541718013421261</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314">
@@ -14200,6 +16082,12 @@
       <c r="N314">
         <v>0.99</v>
       </c>
+      <c r="O314">
+        <v>1.541855029690532</v>
+      </c>
+      <c r="P314">
+        <v>1.541855029690532</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315">
@@ -14244,6 +16132,12 @@
       <c r="N315">
         <v>0.99</v>
       </c>
+      <c r="O315">
+        <v>1.542129503367394</v>
+      </c>
+      <c r="P315">
+        <v>1.542129503367394</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316">
@@ -14288,6 +16182,12 @@
       <c r="N316">
         <v>0.99</v>
       </c>
+      <c r="O316">
+        <v>1.542387110620679</v>
+      </c>
+      <c r="P316">
+        <v>1.542387110620679</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317">
@@ -14332,6 +16232,12 @@
       <c r="N317">
         <v>0.99</v>
       </c>
+      <c r="O317">
+        <v>1.542569546800093</v>
+      </c>
+      <c r="P317">
+        <v>1.542569546800093</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318">
@@ -14376,6 +16282,12 @@
       <c r="N318">
         <v>0.99</v>
       </c>
+      <c r="O318">
+        <v>1.542761414650359</v>
+      </c>
+      <c r="P318">
+        <v>1.542761414650359</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319">
@@ -14420,6 +16332,12 @@
       <c r="N319">
         <v>0.99</v>
       </c>
+      <c r="O319">
+        <v>1.542920025544056</v>
+      </c>
+      <c r="P319">
+        <v>1.542920025544056</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320">
@@ -14464,6 +16382,12 @@
       <c r="N320">
         <v>0.99</v>
       </c>
+      <c r="O320">
+        <v>1.543057858744385</v>
+      </c>
+      <c r="P320">
+        <v>1.543057858744385</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321">
@@ -14508,6 +16432,12 @@
       <c r="N321">
         <v>0.99</v>
       </c>
+      <c r="O321">
+        <v>1.543141435418957</v>
+      </c>
+      <c r="P321">
+        <v>1.543141435418957</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322">
@@ -14552,6 +16482,12 @@
       <c r="N322">
         <v>0.99</v>
       </c>
+      <c r="O322">
+        <v>1.543243333057849</v>
+      </c>
+      <c r="P322">
+        <v>1.543243333057849</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323">
@@ -14596,6 +16532,12 @@
       <c r="N323">
         <v>0.99</v>
       </c>
+      <c r="O323">
+        <v>1.543452331288094</v>
+      </c>
+      <c r="P323">
+        <v>1.543452331288094</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324">
@@ -14640,6 +16582,12 @@
       <c r="N324">
         <v>0.99</v>
       </c>
+      <c r="O324">
+        <v>1.543774460057992</v>
+      </c>
+      <c r="P324">
+        <v>1.543774460057992</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325">
@@ -14684,6 +16632,12 @@
       <c r="N325">
         <v>0.99</v>
       </c>
+      <c r="O325">
+        <v>1.544011099288753</v>
+      </c>
+      <c r="P325">
+        <v>1.544011099288753</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326">
@@ -14728,6 +16682,12 @@
       <c r="N326">
         <v>0.99</v>
       </c>
+      <c r="O326">
+        <v>1.544071374023655</v>
+      </c>
+      <c r="P326">
+        <v>1.544071374023655</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327">
@@ -14772,6 +16732,12 @@
       <c r="N327">
         <v>0.99</v>
       </c>
+      <c r="O327">
+        <v>1.544071374023655</v>
+      </c>
+      <c r="P327">
+        <v>1.544071374023655</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328">
@@ -14816,6 +16782,12 @@
       <c r="N328">
         <v>0.99</v>
       </c>
+      <c r="O328">
+        <v>1.544177070667368</v>
+      </c>
+      <c r="P328">
+        <v>1.544177070667368</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329">
@@ -14860,6 +16832,12 @@
       <c r="N329">
         <v>0.99</v>
       </c>
+      <c r="O329">
+        <v>1.544334023701153</v>
+      </c>
+      <c r="P329">
+        <v>1.544334023701153</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330">
@@ -14904,6 +16882,12 @@
       <c r="N330">
         <v>0.99</v>
       </c>
+      <c r="O330">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P330">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331">
@@ -14948,6 +16932,12 @@
       <c r="N331">
         <v>0.99</v>
       </c>
+      <c r="O331">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P331">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332">
@@ -14992,6 +16982,12 @@
       <c r="N332">
         <v>0.99</v>
       </c>
+      <c r="O332">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P332">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333">
@@ -15036,6 +17032,12 @@
       <c r="N333">
         <v>0.99</v>
       </c>
+      <c r="O333">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P333">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334">
@@ -15080,6 +17082,12 @@
       <c r="N334">
         <v>0.99</v>
       </c>
+      <c r="O334">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P334">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335">
@@ -15124,6 +17132,12 @@
       <c r="N335">
         <v>0.99</v>
       </c>
+      <c r="O335">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P335">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336">
@@ -15168,6 +17182,12 @@
       <c r="N336">
         <v>0.99</v>
       </c>
+      <c r="O336">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P336">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337">
@@ -15212,6 +17232,12 @@
       <c r="N337">
         <v>0.99</v>
       </c>
+      <c r="O337">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P337">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338">
@@ -15256,6 +17282,12 @@
       <c r="N338">
         <v>0.99</v>
       </c>
+      <c r="O338">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P338">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339">
@@ -15300,6 +17332,12 @@
       <c r="N339">
         <v>0.99</v>
       </c>
+      <c r="O339">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P339">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340">
@@ -15344,6 +17382,12 @@
       <c r="N340">
         <v>0.99</v>
       </c>
+      <c r="O340">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P340">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341">
@@ -15388,6 +17432,12 @@
       <c r="N341">
         <v>0.99</v>
       </c>
+      <c r="O341">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P341">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342">
@@ -15432,6 +17482,12 @@
       <c r="N342">
         <v>0.99</v>
       </c>
+      <c r="O342">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P342">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343">
@@ -15476,6 +17532,12 @@
       <c r="N343">
         <v>0.99</v>
       </c>
+      <c r="O343">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P343">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344">
@@ -15520,6 +17582,12 @@
       <c r="N344">
         <v>0.99</v>
       </c>
+      <c r="O344">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P344">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345">
@@ -15564,6 +17632,12 @@
       <c r="N345">
         <v>0.99</v>
       </c>
+      <c r="O345">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P345">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346">
@@ -15608,6 +17682,12 @@
       <c r="N346">
         <v>0.99</v>
       </c>
+      <c r="O346">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P346">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347">
@@ -15652,6 +17732,12 @@
       <c r="N347">
         <v>0.99</v>
       </c>
+      <c r="O347">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P347">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348">
@@ -15696,6 +17782,12 @@
       <c r="N348">
         <v>0.99</v>
       </c>
+      <c r="O348">
+        <v>1.544437607637153</v>
+      </c>
+      <c r="P348">
+        <v>1.544437607637153</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349">
@@ -15740,6 +17832,12 @@
       <c r="N349">
         <v>0.99</v>
       </c>
+      <c r="O349">
+        <v>1.544526706086104</v>
+      </c>
+      <c r="P349">
+        <v>1.544526706086104</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350">
@@ -15784,6 +17882,12 @@
       <c r="N350">
         <v>0.99</v>
       </c>
+      <c r="O350">
+        <v>1.544676074316322</v>
+      </c>
+      <c r="P350">
+        <v>1.544676074316322</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351">
@@ -15828,6 +17932,12 @@
       <c r="N351">
         <v>0.99</v>
       </c>
+      <c r="O351">
+        <v>1.5447969751402</v>
+      </c>
+      <c r="P351">
+        <v>1.5447969751402</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352">
@@ -15872,6 +17982,12 @@
       <c r="N352">
         <v>0.99</v>
       </c>
+      <c r="O352">
+        <v>1.5447969751402</v>
+      </c>
+      <c r="P352">
+        <v>1.5447969751402</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353">
@@ -15916,6 +18032,12 @@
       <c r="N353">
         <v>0.99</v>
       </c>
+      <c r="O353">
+        <v>1.544833683874957</v>
+      </c>
+      <c r="P353">
+        <v>1.544833683874957</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354">
@@ -15960,6 +18082,12 @@
       <c r="N354">
         <v>0.99</v>
       </c>
+      <c r="O354">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P354">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355">
@@ -16004,6 +18132,12 @@
       <c r="N355">
         <v>0.99</v>
       </c>
+      <c r="O355">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P355">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356">
@@ -16048,6 +18182,12 @@
       <c r="N356">
         <v>0.99</v>
       </c>
+      <c r="O356">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P356">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357">
@@ -16092,6 +18232,12 @@
       <c r="N357">
         <v>0.99</v>
       </c>
+      <c r="O357">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P357">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358">
@@ -16136,6 +18282,12 @@
       <c r="N358">
         <v>0.99</v>
       </c>
+      <c r="O358">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P358">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359">
@@ -16180,6 +18332,12 @@
       <c r="N359">
         <v>0.99</v>
       </c>
+      <c r="O359">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P359">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360">
@@ -16224,6 +18382,12 @@
       <c r="N360">
         <v>0.99</v>
       </c>
+      <c r="O360">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P360">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361">
@@ -16268,6 +18432,12 @@
       <c r="N361">
         <v>0.99</v>
       </c>
+      <c r="O361">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P361">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362">
@@ -16312,6 +18482,12 @@
       <c r="N362">
         <v>0.99</v>
       </c>
+      <c r="O362">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P362">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363">
@@ -16356,6 +18532,12 @@
       <c r="N363">
         <v>0.99</v>
       </c>
+      <c r="O363">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P363">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364">
@@ -16400,6 +18582,12 @@
       <c r="N364">
         <v>0.99</v>
       </c>
+      <c r="O364">
+        <v>1.544866961214976</v>
+      </c>
+      <c r="P364">
+        <v>1.544866961214976</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365">
@@ -16444,6 +18632,12 @@
       <c r="N365">
         <v>0.99</v>
       </c>
+      <c r="O365">
+        <v>1.544923327413434</v>
+      </c>
+      <c r="P365">
+        <v>1.544923327413434</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366">
@@ -16487,6 +18681,12 @@
       </c>
       <c r="N366">
         <v>0.99</v>
+      </c>
+      <c r="O366">
+        <v>1.545100670608248</v>
+      </c>
+      <c r="P366">
+        <v>1.545100670608248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>